<commit_message>
[Pipette] Battery Connector 추가 - solder cap type
</commit_message>
<xml_diff>
--- a/1_Plasma_Pipette/4_Review data/Plsma Pipette Review Data.xlsx
+++ b/1_Plasma_Pipette/4_Review data/Plsma Pipette Review Data.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ME Size" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Battery CON" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Battery 용량</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,38 @@
   </si>
   <si>
     <t>Sub</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9155-000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spring</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K113868632</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Top-Link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tyco</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -423,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
@@ -598,12 +630,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F5">
+        <f>D5+E5</f>
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>3.45</v>
+      </c>
+      <c r="E8">
+        <f>4.9-3.45</f>
+        <v>1.4500000000000002</v>
+      </c>
+      <c r="F8">
+        <f>D8+E8</f>
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O12">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O13">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="Q13">
+        <v>0.182</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="O14">
+        <f>O13-O12</f>
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="Q14">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="Q15">
+        <f>Q13-Q14</f>
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>